<commit_message>
Fixes #3119 .  Refactored desorption to put calculations of rates and derivatives into material class instead of kernels.  Added mollified langmuir.  added new tests for original langmuir and mollified version.  altered doco appropriately
</commit_message>
<xml_diff>
--- a/modules/chemical_reactions/doc/desorption/langmuir_test.xlsx
+++ b/modules/chemical_reactions/doc/desorption/langmuir_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="36" windowWidth="17220" windowHeight="10584"/>
+    <workbookView xWindow="288" yWindow="36" windowWidth="17220" windowHeight="10584" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="comparison" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="langmuir_desorption" type="6" refreshedVersion="3" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="L:\moose\project2\trunk\wallaby\tests\kernels\langmuir_desorption.csv" comma="1">
+    <textPr codePage="850" sourceFile="L:\moose\projects_andy\moose\modules\chemical_reactions\tests\desorption\gold\langmuir_desorption.csv" comma="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -24549,11 +24549,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="59753216"/>
-        <c:axId val="59754752"/>
+        <c:axId val="143520128"/>
+        <c:axId val="143522048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="59753216"/>
+        <c:axId val="143520128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -24584,12 +24584,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59754752"/>
+        <c:crossAx val="143522048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59754752"/>
+        <c:axId val="143522048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5"/>
@@ -24622,7 +24622,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59753216"/>
+        <c:crossAx val="143520128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -24640,7 +24640,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="121" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -24966,8 +24966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:M1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>